<commit_message>
extending the createportfolio test
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="82">
   <si>
     <t>TCID</t>
   </si>
@@ -233,6 +233,36 @@
   <si>
     <t>My Portfolio</t>
   </si>
+  <si>
+    <t>createPortfolioTest</t>
+  </si>
+  <si>
+    <t>create_PF_id</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>PF_name_id</t>
+  </si>
+  <si>
+    <t>PF_Name</t>
+  </si>
+  <si>
+    <t>deletePortfolioTest</t>
+  </si>
+  <si>
+    <t>create_PF_btn_id</t>
+  </si>
+  <si>
+    <t>NK2</t>
+  </si>
+  <si>
+    <t>verifyportfolio</t>
+  </si>
+  <si>
+    <t>PF_select_xpath</t>
+  </si>
 </sst>
 </file>
 
@@ -269,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +333,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -368,6 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,7 +766,23 @@
         <v>58</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -740,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM28"/>
+  <dimension ref="A1:AUM44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15955,6 +16008,254 @@
         <v>6</v>
       </c>
     </row>
+    <row r="29" spans="1:1235" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1235" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1235" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1235" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -15963,10 +16264,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16162,7 +16463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -16173,7 +16474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -16184,7 +16485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -16195,12 +16496,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -16217,7 +16518,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -16232,6 +16533,51 @@
       </c>
       <c r="E23" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated from home 17july
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="84">
   <si>
     <t>TCID</t>
   </si>
@@ -195,9 +195,6 @@
     <t>RediffLogin</t>
   </si>
   <si>
-    <t>parvathi8</t>
-  </si>
-  <si>
     <t>rediff_url</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
   </si>
   <si>
     <t>login_ctn_btn_xpath</t>
-  </si>
-  <si>
-    <t>naveen_v20@rediffmail.com</t>
   </si>
   <si>
     <t>pwd_tb_xpath</t>
@@ -235,9 +229,6 @@
   </si>
   <si>
     <t>createPortfolioTest</t>
-  </si>
-  <si>
-    <t>create_PF_id</t>
   </si>
   <si>
     <t>clear</t>
@@ -262,6 +253,21 @@
   </si>
   <si>
     <t>PF_select_xpath</t>
+  </si>
+  <si>
+    <t>Mozilla</t>
+  </si>
+  <si>
+    <t>waitForPageToLoad</t>
+  </si>
+  <si>
+    <t>create_PF_xpath</t>
+  </si>
+  <si>
+    <t>nkuserone</t>
+  </si>
+  <si>
+    <t>King12345</t>
   </si>
 </sst>
 </file>
@@ -771,7 +777,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -779,7 +785,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -793,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM44"/>
+  <dimension ref="A1:AUM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15883,7 +15889,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11" t="s">
@@ -15899,7 +15905,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11" t="s">
@@ -15915,7 +15921,7 @@
         <v>32</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11" t="s">
@@ -15931,7 +15937,7 @@
         <v>33</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>8</v>
@@ -15949,7 +15955,7 @@
         <v>32</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11" t="s">
@@ -15965,7 +15971,7 @@
         <v>33</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>9</v>
@@ -15983,7 +15989,7 @@
         <v>32</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11" t="s">
@@ -15996,13 +16002,13 @@
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>6</v>
@@ -16010,7 +16016,7 @@
     </row>
     <row r="29" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13" t="s">
@@ -16026,14 +16032,14 @@
     </row>
     <row r="30" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13" t="s">
@@ -16042,14 +16048,14 @@
     </row>
     <row r="31" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13" t="s">
@@ -16058,14 +16064,14 @@
     </row>
     <row r="32" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13" t="s">
@@ -16074,14 +16080,14 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>8</v>
@@ -16092,14 +16098,14 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13" t="s">
@@ -16108,14 +16114,14 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>9</v>
@@ -16126,14 +16132,14 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="13" t="s">
@@ -16142,48 +16148,46 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>68</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
       <c r="F37" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="13"/>
+        <v>67</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="F38" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13" t="s">
@@ -16192,32 +16196,28 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>76</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
       <c r="F40" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="13" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="13" t="s">
@@ -16226,35 +16226,85 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="13" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42" s="13"/>
+        <v>73</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
+      <c r="A43" s="13" t="s">
+        <v>70</v>
+      </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="C43" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="F43" s="13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
+      <c r="A44" s="13" t="s">
+        <v>70</v>
+      </c>
       <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
+      <c r="C44" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="F44" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16266,8 +16316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16515,7 +16565,7 @@
         <v>9</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -16526,18 +16576,18 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -16554,10 +16604,10 @@
         <v>9</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -16565,23 +16615,27 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" display="naveen_v20@rediffmail.com"/>
+    <hyperlink ref="C23" r:id="rId2" display="naveen_v20@rediffmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated from offcie delete portfoloi test
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="86">
   <si>
     <t>TCID</t>
   </si>
@@ -252,9 +252,6 @@
     <t>PF_select_xpath</t>
   </si>
   <si>
-    <t>Mozilla</t>
-  </si>
-  <si>
     <t>waitForPageToLoad</t>
   </si>
   <si>
@@ -269,11 +266,20 @@
   <si>
     <t>create_PF_BTN_id_xpath</t>
   </si>
+  <si>
+    <t>PF_delete_Btn_id</t>
+  </si>
+  <si>
+    <t>acceptAlertifpresent</t>
+  </si>
+  <si>
+    <t>dropdownselect</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -305,7 +311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +351,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -411,6 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +484,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -506,7 +519,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,10 +734,10 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -780,7 +793,7 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -788,7 +801,7 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -799,20 +812,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM47"/>
+  <dimension ref="A1:AUM61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1235" x14ac:dyDescent="0.3">
@@ -16152,7 +16165,7 @@
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
@@ -16187,7 +16200,7 @@
         <v>32</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13" t="s">
@@ -16200,7 +16213,7 @@
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -16251,7 +16264,7 @@
         <v>32</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E43" s="13"/>
       <c r="F43" s="13" t="s">
@@ -16264,7 +16277,7 @@
       </c>
       <c r="B44" s="13"/>
       <c r="C44" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
@@ -16291,20 +16304,236 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="A46" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
+      <c r="A47" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16314,18 +16543,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -16576,10 +16805,10 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
         <v>81</v>
-      </c>
-      <c r="D23" t="s">
-        <v>82</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>
@@ -16615,18 +16844,63 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
         <v>81</v>
-      </c>
-      <c r="D27" t="s">
-        <v>82</v>
       </c>
       <c r="E27" t="s">
         <v>69</v>
       </c>
       <c r="F27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
         <v>75</v>
       </c>
     </row>
@@ -16634,8 +16908,9 @@
   <hyperlinks>
     <hyperlink ref="C27" r:id="rId1" display="naveen_v20@rediffmail.com"/>
     <hyperlink ref="C23" r:id="rId2" display="naveen_v20@rediffmail.com"/>
+    <hyperlink ref="C31" r:id="rId3" display="naveen_v20@rediffmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the add del stocl test , needs rework on that
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="87">
   <si>
     <t>TCID</t>
   </si>
@@ -275,11 +275,14 @@
   <si>
     <t>dropdownselect</t>
   </si>
+  <si>
+    <t>addStockTest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +360,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -424,6 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +494,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -519,7 +529,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -728,16 +738,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -801,6 +811,14 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -812,23 +830,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM61"/>
+  <dimension ref="A1:AUM69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59:F67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +866,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -864,7 +882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -880,7 +898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -898,7 +916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -916,7 +934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -932,7 +950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
@@ -946,7 +964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>56</v>
       </c>
@@ -2189,7 +2207,7 @@
       <c r="AUL8"/>
       <c r="AUM8"/>
     </row>
-    <row r="9" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>56</v>
       </c>
@@ -3432,7 +3450,7 @@
       <c r="AUL9"/>
       <c r="AUM9"/>
     </row>
-    <row r="10" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>56</v>
       </c>
@@ -4678,7 +4696,7 @@
       <c r="AUL10"/>
       <c r="AUM10"/>
     </row>
-    <row r="11" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>56</v>
       </c>
@@ -5924,7 +5942,7 @@
       <c r="AUL11"/>
       <c r="AUM11"/>
     </row>
-    <row r="12" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>56</v>
       </c>
@@ -7167,7 +7185,7 @@
       <c r="AUL12"/>
       <c r="AUM12"/>
     </row>
-    <row r="13" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
@@ -8407,7 +8425,7 @@
       <c r="AUL13"/>
       <c r="AUM13"/>
     </row>
-    <row r="14" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>56</v>
       </c>
@@ -9650,7 +9668,7 @@
       <c r="AUL14"/>
       <c r="AUM14"/>
     </row>
-    <row r="15" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>56</v>
       </c>
@@ -10893,7 +10911,7 @@
       <c r="AUL15"/>
       <c r="AUM15"/>
     </row>
-    <row r="16" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>56</v>
       </c>
@@ -12139,7 +12157,7 @@
       <c r="AUL16"/>
       <c r="AUM16"/>
     </row>
-    <row r="17" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
@@ -13385,7 +13403,7 @@
       <c r="AUL17"/>
       <c r="AUM17"/>
     </row>
-    <row r="18" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>56</v>
       </c>
@@ -14631,7 +14649,7 @@
       <c r="AUL18"/>
       <c r="AUM18"/>
     </row>
-    <row r="19" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>56</v>
       </c>
@@ -15877,7 +15895,7 @@
       <c r="AUL19"/>
       <c r="AUM19"/>
     </row>
-    <row r="20" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>58</v>
       </c>
@@ -15893,7 +15911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>58</v>
       </c>
@@ -15909,7 +15927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>58</v>
       </c>
@@ -15925,7 +15943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>58</v>
       </c>
@@ -15941,7 +15959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>58</v>
       </c>
@@ -15959,7 +15977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>58</v>
       </c>
@@ -15975,7 +15993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>58</v>
       </c>
@@ -15993,7 +16011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>58</v>
       </c>
@@ -16009,7 +16027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>58</v>
       </c>
@@ -16027,7 +16045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>70</v>
       </c>
@@ -16043,7 +16061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>70</v>
       </c>
@@ -16059,7 +16077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>70</v>
       </c>
@@ -16075,7 +16093,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:1235" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>70</v>
       </c>
@@ -16091,7 +16109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>70</v>
       </c>
@@ -16109,7 +16127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>70</v>
       </c>
@@ -16125,7 +16143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>70</v>
       </c>
@@ -16143,7 +16161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>70</v>
       </c>
@@ -16159,7 +16177,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>70</v>
       </c>
@@ -16173,7 +16191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>70</v>
       </c>
@@ -16191,7 +16209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>70</v>
       </c>
@@ -16207,7 +16225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>70</v>
       </c>
@@ -16221,7 +16239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>70</v>
       </c>
@@ -16237,7 +16255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>70</v>
       </c>
@@ -16255,7 +16273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>70</v>
       </c>
@@ -16271,7 +16289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>70</v>
       </c>
@@ -16285,7 +16303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>70</v>
       </c>
@@ -16303,7 +16321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>74</v>
       </c>
@@ -16319,7 +16337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>74</v>
       </c>
@@ -16335,7 +16353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>74</v>
       </c>
@@ -16351,7 +16369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>74</v>
       </c>
@@ -16367,7 +16385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>74</v>
       </c>
@@ -16385,7 +16403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
         <v>74</v>
       </c>
@@ -16401,7 +16419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
         <v>74</v>
       </c>
@@ -16419,7 +16437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
         <v>74</v>
       </c>
@@ -16435,7 +16453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
         <v>74</v>
       </c>
@@ -16449,7 +16467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
         <v>74</v>
       </c>
@@ -16467,7 +16485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
         <v>74</v>
       </c>
@@ -16483,7 +16501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="14" t="s">
         <v>74</v>
       </c>
@@ -16497,7 +16515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
         <v>74</v>
       </c>
@@ -16511,29 +16529,171 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16543,26 +16703,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -16579,7 +16739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -16596,7 +16756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -16613,7 +16773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -16630,12 +16790,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -16664,7 +16824,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -16693,7 +16853,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -16704,12 +16864,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
@@ -16723,7 +16883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -16737,12 +16897,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -16753,7 +16913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -16764,7 +16924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -16775,12 +16935,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -16797,7 +16957,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -16814,12 +16974,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>1</v>
       </c>
@@ -16839,7 +16999,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -16859,12 +17019,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -16884,7 +17044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -16901,6 +17061,51 @@
         <v>69</v>
       </c>
       <c r="F31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" t="s">
         <v>75</v>
       </c>
     </row>
@@ -16909,8 +17114,9 @@
     <hyperlink ref="C27" r:id="rId1" display="naveen_v20@rediffmail.com"/>
     <hyperlink ref="C23" r:id="rId2" display="naveen_v20@rediffmail.com"/>
     <hyperlink ref="C31" r:id="rId3" display="naveen_v20@rediffmail.com"/>
+    <hyperlink ref="C35" r:id="rId4" display="naveen_v20@rediffmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added from home , add or del stock
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="100">
   <si>
     <t>TCID</t>
   </si>
@@ -278,6 +278,45 @@
   <si>
     <t>addStockTest</t>
   </si>
+  <si>
+    <t>Ashi_29</t>
+  </si>
+  <si>
+    <t>add_stock_btn_id</t>
+  </si>
+  <si>
+    <t>add_stock_name_id</t>
+  </si>
+  <si>
+    <t>stock_name</t>
+  </si>
+  <si>
+    <t>Tata Steel Ltd</t>
+  </si>
+  <si>
+    <t>result_stock_xpath</t>
+  </si>
+  <si>
+    <t>selectDateddMMyyyy</t>
+  </si>
+  <si>
+    <t>stk_buy_date</t>
+  </si>
+  <si>
+    <t>12/04/2017</t>
+  </si>
+  <si>
+    <t>ad_stock_quantity_id</t>
+  </si>
+  <si>
+    <t>stk_price_id</t>
+  </si>
+  <si>
+    <t>stk_price</t>
+  </si>
+  <si>
+    <t>stock_puchase_date_id</t>
+  </si>
 </sst>
 </file>
 
@@ -417,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -434,6 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,10 +870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM69"/>
+  <dimension ref="A1:AUM79"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:F67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16680,20 +16720,186 @@
         <v>86</v>
       </c>
       <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
+      <c r="C68" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>86</v>
       </c>
       <c r="B69" s="15"/>
-      <c r="C69" s="15"/>
+      <c r="C69" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
+      <c r="F69" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16706,7 +16912,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16715,6 +16921,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
@@ -17064,12 +17271,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>1</v>
       </c>
@@ -17088,8 +17295,17 @@
       <c r="F34" s="12" t="s">
         <v>73</v>
       </c>
+      <c r="G34" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -17106,7 +17322,16 @@
         <v>69</v>
       </c>
       <c r="F35" t="s">
-        <v>75</v>
+        <v>87</v>
+      </c>
+      <c r="G35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
coorected the data files for add or del stock test
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Keywords" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="102">
   <si>
     <t>TCID</t>
   </si>
@@ -309,19 +309,25 @@
     <t>ad_stock_quantity_id</t>
   </si>
   <si>
-    <t>stk_price_id</t>
-  </si>
-  <si>
     <t>stk_price</t>
   </si>
   <si>
     <t>stock_puchase_date_id</t>
   </si>
+  <si>
+    <t>stk_quantity</t>
+  </si>
+  <si>
+    <t>stk_price_xpath</t>
+  </si>
+  <si>
+    <t>stk_add_button_xpath</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -534,7 +540,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -569,7 +575,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -784,10 +790,10 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -870,23 +876,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM79"/>
+  <dimension ref="A1:AUM78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +912,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -922,7 +928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -938,7 +944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -956,7 +962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -974,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -990,7 +996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>56</v>
       </c>
@@ -2247,7 +2253,7 @@
       <c r="AUL8"/>
       <c r="AUM8"/>
     </row>
-    <row r="9" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>56</v>
       </c>
@@ -3490,7 +3496,7 @@
       <c r="AUL9"/>
       <c r="AUM9"/>
     </row>
-    <row r="10" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>56</v>
       </c>
@@ -4736,7 +4742,7 @@
       <c r="AUL10"/>
       <c r="AUM10"/>
     </row>
-    <row r="11" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>56</v>
       </c>
@@ -5982,7 +5988,7 @@
       <c r="AUL11"/>
       <c r="AUM11"/>
     </row>
-    <row r="12" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>56</v>
       </c>
@@ -7225,7 +7231,7 @@
       <c r="AUL12"/>
       <c r="AUM12"/>
     </row>
-    <row r="13" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
@@ -8465,7 +8471,7 @@
       <c r="AUL13"/>
       <c r="AUM13"/>
     </row>
-    <row r="14" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>56</v>
       </c>
@@ -9708,7 +9714,7 @@
       <c r="AUL14"/>
       <c r="AUM14"/>
     </row>
-    <row r="15" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>56</v>
       </c>
@@ -10951,7 +10957,7 @@
       <c r="AUL15"/>
       <c r="AUM15"/>
     </row>
-    <row r="16" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>56</v>
       </c>
@@ -12197,7 +12203,7 @@
       <c r="AUL16"/>
       <c r="AUM16"/>
     </row>
-    <row r="17" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
@@ -13443,7 +13449,7 @@
       <c r="AUL17"/>
       <c r="AUM17"/>
     </row>
-    <row r="18" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>56</v>
       </c>
@@ -14689,7 +14695,7 @@
       <c r="AUL18"/>
       <c r="AUM18"/>
     </row>
-    <row r="19" spans="1:1235" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1235" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>56</v>
       </c>
@@ -15935,7 +15941,7 @@
       <c r="AUL19"/>
       <c r="AUM19"/>
     </row>
-    <row r="20" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>58</v>
       </c>
@@ -15951,7 +15957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>58</v>
       </c>
@@ -15967,7 +15973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>58</v>
       </c>
@@ -15983,7 +15989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>58</v>
       </c>
@@ -15999,7 +16005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>58</v>
       </c>
@@ -16017,7 +16023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>58</v>
       </c>
@@ -16033,7 +16039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>58</v>
       </c>
@@ -16051,7 +16057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>58</v>
       </c>
@@ -16067,7 +16073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>58</v>
       </c>
@@ -16085,7 +16091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>70</v>
       </c>
@@ -16101,7 +16107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>70</v>
       </c>
@@ -16117,7 +16123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>70</v>
       </c>
@@ -16133,7 +16139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:1235" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1235" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>70</v>
       </c>
@@ -16149,7 +16155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>70</v>
       </c>
@@ -16167,7 +16173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>70</v>
       </c>
@@ -16183,7 +16189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>70</v>
       </c>
@@ -16201,7 +16207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>70</v>
       </c>
@@ -16217,7 +16223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>70</v>
       </c>
@@ -16231,7 +16237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>70</v>
       </c>
@@ -16249,7 +16255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>70</v>
       </c>
@@ -16265,7 +16271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>70</v>
       </c>
@@ -16279,7 +16285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>70</v>
       </c>
@@ -16295,7 +16301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>70</v>
       </c>
@@ -16313,7 +16319,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>70</v>
       </c>
@@ -16329,7 +16335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>70</v>
       </c>
@@ -16343,7 +16349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>70</v>
       </c>
@@ -16361,7 +16367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>74</v>
       </c>
@@ -16377,7 +16383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>74</v>
       </c>
@@ -16393,7 +16399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>74</v>
       </c>
@@ -16409,7 +16415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>74</v>
       </c>
@@ -16425,7 +16431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>74</v>
       </c>
@@ -16443,7 +16449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
         <v>74</v>
       </c>
@@ -16459,7 +16465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
         <v>74</v>
       </c>
@@ -16477,7 +16483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
         <v>74</v>
       </c>
@@ -16493,7 +16499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
         <v>74</v>
       </c>
@@ -16507,7 +16513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
         <v>74</v>
       </c>
@@ -16525,7 +16531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
         <v>74</v>
       </c>
@@ -16541,7 +16547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="14" t="s">
         <v>74</v>
       </c>
@@ -16555,7 +16561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
         <v>74</v>
       </c>
@@ -16569,7 +16575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>86</v>
       </c>
@@ -16585,7 +16591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>86</v>
       </c>
@@ -16601,7 +16607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>86</v>
       </c>
@@ -16617,7 +16623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
         <v>86</v>
       </c>
@@ -16633,7 +16639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
         <v>86</v>
       </c>
@@ -16651,7 +16657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="15" t="s">
         <v>86</v>
       </c>
@@ -16667,7 +16673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
         <v>86</v>
       </c>
@@ -16685,7 +16691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="15" t="s">
         <v>86</v>
       </c>
@@ -16701,7 +16707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>86</v>
       </c>
@@ -16715,7 +16721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>86</v>
       </c>
@@ -16733,7 +16739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>86</v>
       </c>
@@ -16747,7 +16753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="15" t="s">
         <v>86</v>
       </c>
@@ -16763,7 +16769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>86</v>
       </c>
@@ -16781,7 +16787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
         <v>86</v>
       </c>
@@ -16797,7 +16803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
         <v>86</v>
       </c>
@@ -16806,12 +16812,12 @@
         <v>32</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E73" s="15"/>
       <c r="F73" s="15"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>86</v>
       </c>
@@ -16827,23 +16833,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
         <v>86</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E75" s="15"/>
+        <v>100</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="F75" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>86</v>
       </c>
@@ -16852,16 +16860,16 @@
         <v>33</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F76" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>86</v>
       </c>
@@ -16870,14 +16878,14 @@
         <v>32</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E77" s="15"/>
       <c r="F77" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>86</v>
       </c>
@@ -16890,16 +16898,6 @@
       <c r="F78" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16909,27 +16907,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -16946,7 +16944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -16963,7 +16961,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -16980,7 +16978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -16997,12 +16995,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -17031,7 +17029,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -17060,7 +17058,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -17071,12 +17069,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
@@ -17090,7 +17088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -17104,12 +17102,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -17120,7 +17118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -17131,7 +17129,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -17142,12 +17140,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -17164,7 +17162,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -17181,12 +17179,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>1</v>
       </c>
@@ -17206,7 +17204,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -17226,12 +17224,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -17251,7 +17249,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -17271,12 +17269,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>1</v>
       </c>
@@ -17302,10 +17300,13 @@
         <v>94</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -17333,15 +17334,12 @@
       <c r="I35">
         <v>120</v>
       </c>
+      <c r="J35">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C27" r:id="rId1" display="naveen_v20@rediffmail.com"/>
-    <hyperlink ref="C23" r:id="rId2" display="naveen_v20@rediffmail.com"/>
-    <hyperlink ref="C31" r:id="rId3" display="naveen_v20@rediffmail.com"/>
-    <hyperlink ref="C35" r:id="rId4" display="naveen_v20@rediffmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added from ofc del stock test
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/rediff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="105">
   <si>
     <t>TCID</t>
   </si>
@@ -322,6 +322,15 @@
   </si>
   <si>
     <t>stk_add_button_xpath</t>
+  </si>
+  <si>
+    <t>redmoney_addstk_succ</t>
+  </si>
+  <si>
+    <t>deleteStockTest</t>
+  </si>
+  <si>
+    <t>deletestockontable</t>
   </si>
 </sst>
 </file>
@@ -784,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,6 +877,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -876,15 +893,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AUM78"/>
+  <dimension ref="A1:AUM91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" customWidth="1"/>
@@ -16657,7 +16674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
         <v>86</v>
       </c>
@@ -16673,7 +16690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>86</v>
       </c>
@@ -16691,7 +16708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>86</v>
       </c>
@@ -16707,7 +16724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>86</v>
       </c>
@@ -16721,7 +16738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>86</v>
       </c>
@@ -16739,7 +16756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>86</v>
       </c>
@@ -16753,7 +16770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
         <v>86</v>
       </c>
@@ -16769,7 +16786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>86</v>
       </c>
@@ -16787,7 +16804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
         <v>86</v>
       </c>
@@ -16803,7 +16820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>86</v>
       </c>
@@ -16815,9 +16832,11 @@
         <v>98</v>
       </c>
       <c r="E73" s="15"/>
-      <c r="F73" s="15"/>
+      <c r="F73" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="74" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>86</v>
       </c>
@@ -16833,7 +16852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>86</v>
       </c>
@@ -16851,7 +16870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>86</v>
       </c>
@@ -16869,7 +16888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
         <v>86</v>
       </c>
@@ -16885,7 +16904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
         <v>86</v>
       </c>
@@ -16896,6 +16915,216 @@
       <c r="D78" s="15"/>
       <c r="E78" s="15"/>
       <c r="F78" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F91" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -16907,10 +17136,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17338,6 +17567,75 @@
         <v>20</v>
       </c>
     </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39">
+        <v>120</v>
+      </c>
+      <c r="J39">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>